<commit_message>
Updated cequing account file
</commit_message>
<xml_diff>
--- a/tests/A02_pixell_test_plan_chequing_account.xlsx
+++ b/tests/A02_pixell_test_plan_chequing_account.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Intermediate Software Development0315\2. Assignments\assignments\assignment_02\instructions\given_files\assignment_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rrcca-my.sharepoint.com/personal/karanveersingh7_rrc_ca/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2873F10E-F8B1-4F89-8CDF-A98B96DD770E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{6E06AC3C-4777-40B0-AE9E-0DFE579C751C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{035971F5-AB3F-432B-8F32-0A88FCFDF79C}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="3555" windowWidth="25185" windowHeight="11415" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="1100" yWindow="1100" windowWidth="19200" windowHeight="11170" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="43">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -249,6 +249,69 @@
   </si>
   <si>
     <t>Attributes are set to input values (ensure to test for superclass and subclass attributes)</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Account is created with a balance greater than the overdraft limit</t>
+  </si>
+  <si>
+    <t>Account is created with a balance less thatn the overdraft limit</t>
+  </si>
+  <si>
+    <t>Account is created with a balance equal to the overdraft limit</t>
+  </si>
+  <si>
+    <t>Account is created with specific values</t>
+  </si>
+  <si>
+    <t>account_number = 112233, client_number = 889900, balance = 500, date_created = date.today(), overdraft_limit = -100, overdraft_rate = 0.05</t>
+  </si>
+  <si>
+    <t>account_number = 112233, client_number = 889900, balance = 500, date_created = date.today(), overdraft_limit = "invalid", overdraft_rate = 0.05</t>
+  </si>
+  <si>
+    <t>account_number = 112233, client_number = 889900, balance = 500, date_created = date.today(), overdraft_limit = -100, overdraft_rate = "invalid"</t>
+  </si>
+  <si>
+    <t>account_number = 112233, client_number = 889900, balance = 500, date_created = "invalid date", overdraft_limit = -100, overdraft_rate = 0.05</t>
+  </si>
+  <si>
+    <t>balance = 0, overdraft_limit = -100, overdraft_rate = 0.05</t>
+  </si>
+  <si>
+    <t>balance = -600, overdraft_limit = -100, overdraft_rate = 0.05</t>
+  </si>
+  <si>
+    <t>balance = -100, overdraft_limit = -100, overdraft_rate = 0.05</t>
+  </si>
+  <si>
+    <t>account_number = 112233, client_number = 889900, balance = 1559.49, date_created=date.today(), overdraft_limit = -15.00, overdraft_rate = 0.05</t>
+  </si>
+  <si>
+    <t>Account initialized with correct attribute values.</t>
+  </si>
+  <si>
+    <t>Overdraft limit is set to default value which is -100 or raises a ValueError.</t>
+  </si>
+  <si>
+    <t>Overdraft rate is set to default value which is 0.05 or raises a ValueError.</t>
+  </si>
+  <si>
+    <t>Raises ValueError for invalid date type.</t>
+  </si>
+  <si>
+    <t>Total service charges calculated = $0.50</t>
+  </si>
+  <si>
+    <t>Total service charges calculated as $0.50 + (amount over limit * rate).</t>
+  </si>
+  <si>
+    <t>Total service charges calculated as $0.50.</t>
+  </si>
+  <si>
+    <t>Returns string: "Account Number: 112233 Balance: $1,559.49\nOverdraft Limit: $-15.00 Overdraft Rate: 5.00% Account Type: Chequing"</t>
   </si>
 </sst>
 </file>
@@ -1154,22 +1217,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="B1:G32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="48.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="4" max="4" width="32.7265625" customWidth="1"/>
+    <col min="5" max="5" width="31.54296875" customWidth="1"/>
+    <col min="6" max="6" width="28.26953125" customWidth="1"/>
+    <col min="7" max="7" width="48.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="2.15">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -1181,14 +1244,14 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1197,10 +1260,10 @@
       </c>
       <c r="D4" s="19"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="11">
         <v>1</v>
       </c>
@@ -1230,11 +1293,17 @@
       <c r="D7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="3">
         <v>2</v>
       </c>
@@ -1244,11 +1313,17 @@
       <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="11">
         <v>3</v>
       </c>
@@ -1258,11 +1333,17 @@
       <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="11">
         <v>4</v>
       </c>
@@ -1272,11 +1353,17 @@
       <c r="D10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="3">
         <v>5</v>
       </c>
@@ -1286,11 +1373,17 @@
       <c r="D11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="11">
         <v>6</v>
       </c>
@@ -1300,11 +1393,17 @@
       <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="11">
         <v>7</v>
       </c>
@@ -1314,11 +1413,17 @@
       <c r="D13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="2:7" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="3">
         <v>8</v>
       </c>
@@ -1328,11 +1433,17 @@
       <c r="D14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="11">
         <v>9</v>
       </c>
@@ -1342,7 +1453,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="11">
         <v>10</v>
       </c>
@@ -1352,7 +1463,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="3">
         <v>11</v>
       </c>
@@ -1362,7 +1473,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="11">
         <v>12</v>
       </c>
@@ -1372,7 +1483,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="11">
         <v>13</v>
       </c>
@@ -1382,7 +1493,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="3">
         <v>14</v>
       </c>
@@ -1392,7 +1503,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="11">
         <v>15</v>
       </c>
@@ -1402,7 +1513,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="11">
         <v>16</v>
       </c>
@@ -1412,7 +1523,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="3">
         <v>17</v>
       </c>
@@ -1422,7 +1533,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="11">
         <v>18</v>
       </c>
@@ -1432,7 +1543,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="11">
         <v>19</v>
       </c>
@@ -1442,7 +1553,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="3">
         <v>20</v>
       </c>
@@ -1452,7 +1563,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="11">
         <v>21</v>
       </c>
@@ -1462,7 +1573,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="11">
         <v>22</v>
       </c>
@@ -1472,7 +1583,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="3">
         <v>23</v>
       </c>
@@ -1482,7 +1593,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="11">
         <v>24</v>
       </c>
@@ -1492,7 +1603,7 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B32" s="20" t="s">
         <v>6</v>
       </c>
@@ -1515,4 +1626,292 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009BE1E6CA44A20B4E831DF318AD475E14" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c5b3a412bdb16e09277d0befc7f04846">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="89554b47-2552-4b86-8593-c795689c0073" xmlns:ns4="aeff4388-0e26-4e3c-88c8-6ffddba0a797" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="28028d0dfdec3718c79b693512d4d155" ns3:_="" ns4:_="">
+    <xsd:import namespace="89554b47-2552-4b86-8593-c795689c0073"/>
+    <xsd:import namespace="aeff4388-0e26-4e3c-88c8-6ffddba0a797"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="89554b47-2552-4b86-8593-c795689c0073" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_activity" ma:index="11" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="15" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSystemTags" ma:index="16" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="17" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="18" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="19" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="20" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="21" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="aeff4388-0e26-4e3c-88c8-6ffddba0a797" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="14" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="89554b47-2552-4b86-8593-c795689c0073" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01795345-9744-4BAA-BD2A-6F88DFF2393C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="89554b47-2552-4b86-8593-c795689c0073"/>
+    <ds:schemaRef ds:uri="aeff4388-0e26-4e3c-88c8-6ffddba0a797"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FFF7420-E4AA-4F18-BA7C-CBC69261046E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75865715-524A-43D3-9979-1F87202B23C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="aeff4388-0e26-4e3c-88c8-6ffddba0a797"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="89554b47-2552-4b86-8593-c795689c0073"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>